<commit_message>
Update Lab2-FSM-Table - Alberto MJ.xlsx
</commit_message>
<xml_diff>
--- a/Assets/Scripts/Lab 2/Lab2-FSM-Table - Alberto MJ.xlsx
+++ b/Assets/Scripts/Lab 2/Lab2-FSM-Table - Alberto MJ.xlsx
@@ -2,41 +2,30 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CENTENNIAL\F2024\COMP-Classes\Labs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alber\Desktop\Codes\GameProgramming2\Assets\Scripts\Lab 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C238EF35-690F-4D81-BD12-0B1E263AD3D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06371EE5-2DF4-474B-9C68-3E7C91E208AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5F90E7CF-4FC2-410E-BFE2-5069794AA61B}"/>
+    <workbookView xWindow="2040" yWindow="1095" windowWidth="21600" windowHeight="11385" xr2:uid="{5F90E7CF-4FC2-410E-BFE2-5069794AA61B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>State</t>
   </si>
@@ -84,6 +73,27 @@
   </si>
   <si>
     <t>Distance to player is bigger then 5</t>
+  </si>
+  <si>
+    <t>DefendHq</t>
+  </si>
+  <si>
+    <t>ReturnToHq</t>
+  </si>
+  <si>
+    <t>StopChasing</t>
+  </si>
+  <si>
+    <t>Player distance to hq is less than 5 and guard distance to hq is less than 5</t>
+  </si>
+  <si>
+    <t>Guard distance to hq is more than 15</t>
+  </si>
+  <si>
+    <t>Player distance to guard is more than 15</t>
+  </si>
+  <si>
+    <t>FleeToHq</t>
   </si>
 </sst>
 </file>
@@ -498,7 +508,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,19 +607,37 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="10" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="11" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="12" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A12" s="1"/>

</xml_diff>